<commit_message>
Changed j:Subject to j:BookingSubject.  Updated mapping spreadsheet.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1180" windowWidth="31900" windowHeight="16200"/>
+    <workbookView xWindow="3320" yWindow="260" windowWidth="31900" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Business</t>
   </si>
@@ -96,18 +96,6 @@
     <t>Consent Decision Code</t>
   </si>
   <si>
-    <t>/cdr-doc:ConsentDecisionReport/j:Booking[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/j:BookingAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/j:Booking[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionCode</t>
-  </si>
-  <si>
     <t>/cdr-doc:ConsentDecisionReport/nc:DocumentFileControlID</t>
   </si>
   <si>
@@ -123,21 +111,6 @@
     <t>Consent Notes</t>
   </si>
   <si>
-    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Subject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Subject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Subject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Subject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Subject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
-  </si>
-  <si>
     <t>Document ID</t>
   </si>
   <si>
@@ -150,16 +123,61 @@
     <t>/cdr-doc:ConsentDecisionReport/nc:DocumentCreationDate/nc:Date</t>
   </si>
   <si>
-    <t>/cdr-doc:ConsentDecisionReport/j:Subject/j:SubjectIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/j:Booking[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Subject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/j:ActivityAugmentation/j:Narrative/nc:CommentText</t>
+    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking/j:BookingAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/j:ActivityAugmentation/j:Narrative/nc:CommentText</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionCode</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionRecordingEntity/nc:EntityPerson/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionRecordingEntity/nc:EntityPerson/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionRecordingEntity/cdr-ext:RecordingEntityUsernameText</t>
+  </si>
+  <si>
+    <t>Consent Recording Person First Name</t>
+  </si>
+  <si>
+    <t>Consent Recording Person Last Name</t>
+  </si>
+  <si>
+    <t>Consent Recording Person Username</t>
   </si>
 </sst>
 </file>
@@ -711,7 +729,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -774,6 +792,32 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -819,6 +863,18 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -828,20 +884,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -880,6 +924,19 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -895,6 +952,19 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1202,13 +1272,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1221,19 +1291,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" hidden="1" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
@@ -1252,45 +1322,45 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" ht="15">
-      <c r="A4" s="21" t="s">
-        <v>41</v>
+      <c r="A4" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" s="20" customFormat="1">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:4" s="17" customFormat="1">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" s="20" customFormat="1">
-      <c r="A6" s="18" t="s">
-        <v>39</v>
+    <row r="6" spans="1:4" s="17" customFormat="1">
+      <c r="A6" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" s="20" customFormat="1">
-      <c r="A7" s="18" t="s">
-        <v>30</v>
+    <row r="7" spans="1:4" s="17" customFormat="1">
+      <c r="A7" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" ht="15">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="12"/>
@@ -1298,7 +1368,7 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="13"/>
@@ -1342,51 +1412,51 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="15">
-      <c r="A15" s="21" t="s">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="15">
+      <c r="A14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" s="19" customFormat="1" ht="28">
-      <c r="A16" s="19" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="16" customFormat="1">
+      <c r="A16" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="19" customFormat="1" ht="28">
-      <c r="A17" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="16" customFormat="1">
+      <c r="A17" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="19" customFormat="1" ht="28">
-      <c r="A18" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="16" customFormat="1">
+      <c r="A18" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="5" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="12"/>
@@ -1394,63 +1464,84 @@
     </row>
     <row r="20" spans="1:3" s="6" customFormat="1" ht="28">
       <c r="A20" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="6" customFormat="1" ht="28">
       <c r="A21" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="19" customFormat="1" ht="28">
-      <c r="A22" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="16" customFormat="1" ht="28">
+      <c r="A22" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="19" customFormat="1" ht="28">
-      <c r="A23" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="16" customFormat="1" ht="28">
+      <c r="A23" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="19" customFormat="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="16" customFormat="1">
       <c r="B24" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" s="19" customFormat="1">
+    <row r="25" spans="1:3" s="16" customFormat="1">
       <c r="B25" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:3" s="19" customFormat="1">
+    <row r="26" spans="1:3" s="16" customFormat="1">
       <c r="B26" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" s="19" customFormat="1">
+    <row r="27" spans="1:3" s="16" customFormat="1" ht="28">
+      <c r="A27" s="16" t="s">
+        <v>50</v>
+      </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
+      <c r="C27" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28">
+      <c r="A28" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28">
+      <c r="A29" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Removed ActivityPersonAssociation.  Updated cardinality and mapping.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="260" windowWidth="31900" windowHeight="16200"/>
+    <workbookView xWindow="-27900" yWindow="300" windowWidth="31900" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -150,27 +150,6 @@
     <t>/br-doc:BookingReport/j:Booking/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/j:ActivityAugmentation/j:Narrative/nc:CommentText</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionCode</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionRecordingEntity/nc:EntityPerson/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionRecordingEntity/nc:EntityPerson/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision[@structures:id=../nc:ActivityPersonAssociation[nc:Person/@structures:ref=/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:Activity/@structures:ref]/cdr-ext:ConsentDecisionRecordingEntity/cdr-ext:RecordingEntityUsernameText</t>
-  </si>
-  <si>
     <t>Consent Recording Person First Name</t>
   </si>
   <si>
@@ -178,6 +157,27 @@
   </si>
   <si>
     <t>Consent Recording Person Username</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/j:ActivityAugmentation/j:Narrative/nc:CommentText</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/cdr-ext:ConsentDecisionCode</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/cdr-ext:ConsentDecisionRecordingEntity/nc:EntityPerson/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/cdr-ext:ConsentDecisionRecordingEntity/nc:EntityPerson/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/cdr-ext:ConsentDecisionRecordingEntity/cdr-ext:RecordingEntityUsernameText</t>
   </si>
 </sst>
 </file>
@@ -1274,11 +1274,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1462,34 +1462,34 @@
       <c r="B19" s="12"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" s="6" customFormat="1" ht="28">
+    <row r="20" spans="1:3" s="6" customFormat="1">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="6" customFormat="1" ht="28">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="6" customFormat="1">
       <c r="A21" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="16" customFormat="1" ht="28">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="16" customFormat="1">
       <c r="A22" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="16" customFormat="1" ht="28">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="16" customFormat="1">
       <c r="A23" s="16" t="s">
         <v>24</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="16" customFormat="1">
@@ -1518,29 +1518,29 @@
       </c>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" s="16" customFormat="1" ht="28">
+    <row r="27" spans="1:3" s="16" customFormat="1">
       <c r="A27" s="16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="28">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Consent codes to "2" codes.  Removed Facility Name/Number.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27900" yWindow="300" windowWidth="31900" windowHeight="16200"/>
+    <workbookView xWindow="6800" yWindow="1580" windowWidth="31900" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Business</t>
   </si>
@@ -66,24 +66,6 @@
     <t>Document Control Number</t>
   </si>
   <si>
-    <t>Consent Granted</t>
-  </si>
-  <si>
-    <t>Consent Denied</t>
-  </si>
-  <si>
-    <t>Inmate Never Seen</t>
-  </si>
-  <si>
-    <t>Consent Not Obtained</t>
-  </si>
-  <si>
-    <t>Booking Facility Name</t>
-  </si>
-  <si>
-    <t>Booking Facility Number</t>
-  </si>
-  <si>
     <t>Booking</t>
   </si>
   <si>
@@ -141,12 +123,6 @@
     <t>/br-doc:BookingReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Booking/j:BookingAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Booking/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/br-doc:BookingReport/j:Booking/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -178,6 +154,9 @@
   </si>
   <si>
     <t>/cdr-doc:ConsentDecisionReport/cdr-ext:ConsentDecision/cdr-ext:ConsentDecisionRecordingEntity/cdr-ext:RecordingEntityUsernameText</t>
+  </si>
+  <si>
+    <t>Codes: Consent Granted; Consent Denied</t>
   </si>
 </sst>
 </file>
@@ -729,7 +708,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -818,6 +797,8 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -885,7 +866,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="90">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -937,6 +918,7 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -965,6 +947,7 @@
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1272,13 +1255,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1323,7 +1306,7 @@
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" ht="15">
       <c r="A4" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="3"/>
@@ -1335,27 +1318,27 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1">
       <c r="A6" s="15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1">
       <c r="A7" s="15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D7" s="6"/>
     </row>
@@ -1373,7 +1356,7 @@
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1">
@@ -1382,7 +1365,7 @@
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17" customHeight="1">
@@ -1391,7 +1374,7 @@
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16.5" customHeight="1">
@@ -1400,7 +1383,7 @@
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1">
@@ -1409,23 +1392,23 @@
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="15">
       <c r="A14" s="18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="16" customFormat="1">
@@ -1434,113 +1417,77 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="16" customFormat="1">
-      <c r="A17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" s="6" customFormat="1">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="6" customFormat="1">
+      <c r="A19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="16" customFormat="1">
-      <c r="A18" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="5" t="s">
+    <row r="20" spans="1:3" s="16" customFormat="1">
+      <c r="A20" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="16" customFormat="1">
+      <c r="A21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" s="6" customFormat="1">
-      <c r="A20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="6" customFormat="1">
-      <c r="A21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="16" customFormat="1">
       <c r="A22" s="16" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="16" customFormat="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="16" customFormat="1">
-      <c r="B24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="10"/>
-    </row>
-    <row r="25" spans="1:3" s="16" customFormat="1">
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" s="16" customFormat="1">
-      <c r="B26" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" s="16" customFormat="1">
-      <c r="A27" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="16" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated mapping of SubjectID and RecordID
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Consent_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="1580" windowWidth="31900" windowHeight="16200"/>
+    <workbookView xWindow="5960" yWindow="3500" windowWidth="31900" windowHeight="16200"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -120,12 +120,6 @@
     <t>/cdr-doc:ConsentDecisionReport/nc:Person[@structures:id=../j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
   </si>
   <si>
-    <t>/br-doc:BookingReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReport/j:Booking/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>Consent Recording Person First Name</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>Codes: Consent Granted; Consent Denied</t>
+  </si>
+  <si>
+    <t>/cdr-doc:ConsentDecisionReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>cdr-doc:ConsentDecisionReport/j:Booking/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1261,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="16" customFormat="1">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="5" customFormat="1" ht="15">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="16" customFormat="1">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="16" customFormat="1">
@@ -1459,35 +1459,35 @@
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="16" customFormat="1">
       <c r="A22" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>